<commit_message>
feat: enhance analyzer to support English-to-Chinese summary and extra fields
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,65 +434,85 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Authors</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Background</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Significance</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Logic</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Methodology</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Conclusions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Dep. Var</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Indep. Var</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Mechanism</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Instrumental</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Controls</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Data Source</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Measurements</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>References (Top 5)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
         <is>
           <t>Stata Code</t>
         </is>
@@ -501,324 +521,507 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>休闲农业与乡村旅游发展促进...？——来自准自然实验的证据_黄祖辉.pdf</t>
+          <t>1-QJE-原神论文.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>休闲农业与乡村旅游发展促进农民增收了吗？——来自准自然实验的证据</t>
+          <t>数字分心与同伴影响：移动应用使用对学术和劳动市场结果的影响</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>休闲农业与乡村旅游作为推进农村产业融合发展的新载体，是带动农民增收致富的“绿色”驱动力。文章借助全国休闲农业与乡村旅游示范县政策的“准自然实验”，采用2005-2018年中国816个县的面板数据和多期方法，实证检验了休闲农业与乡村旅游发展对农民增收的影响、作用机理和制约因素。</t>
+          <t>Panle Jia Barwick, Siyu Chen, Chao Fu, Teng Li</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>研究不仅提供了大力发展休闲农业与乡村旅游的重要实践基础，也为促进乡村振兴和实现共同富裕提供了政策启示。</t>
+          <t>Quarterly Journal of Economics</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>研究首先通过PSM方法匹配示范县和非示范县，构建反事实框架，降低样本选择偏误。然后利用DID方法估计示范县政策的增收效应，并进行平行趋势检验确保模型的有效性。进一步，通过加入中介变量检验增收的具体作用机理，包括就业效应和技术效应。最后，通过异质性分析探讨不同条件下示范县政策的增收效果。</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1. 使用PSM方法匹配示范县和非示范县，构建反事实框架。2. 利用DID方法估计示范县政策的增收效应。3. 进行平行趋势检验确保模型的有效性。4. 通过加入中介变量检验增收的具体作用机理。5. 通过异质性分析探讨不同条件下示范县政策的增收效果。</t>
+          <t>随着对手机过度使用的担忧日益增加，尤其是在青少年和年轻人中，本研究提供了首个关于个人及同伴移动应用使用对学术表现、身体健康和劳动市场结果影响的综合证据。研究利用中国一所大学的行政数据和手机记录，通过随机室友分配和政策冲击，探讨了个人及同伴的移动应用使用对学术成绩、身体健康和劳动市场结果的影响。</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['全国休闲农业与乡村旅游示范县政策显著提高了农村居民人均纯收入和收入增长率。', '政策的增收效应随时间推移越来越强。', '在乡村旅游资源禀赋越好、经济发展水平越高的地区，政策的增收效应能够得到更大程度的发挥。', '乡村非农就业水平提升和农业技术采用增加是示范县政策发挥增收效应的重要渠道。']</t>
+          <t>本研究不仅在理论上增进了对数字分心和同伴效应的理解，而且在实践上为制定相关政策提供了依据，如限制青少年手机使用时间的政策可能会对他们未来的劳动市场结果产生积极影响。</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>农村居民人均纯收入及其增长率</t>
+          <t>研究首先通过随机室友分配来估计同伴效应，然后利用政策变化作为工具变量来分离行为溢出效应和情境同伴效应，最后探讨了移动应用使用对学术成绩和劳动市场结果的影响。</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>全国休闲农业与乡村旅游示范县政策</t>
+          <t>研究者首先利用随机室友分配来估计同伴效应，然后通过政策变化作为工具变量来分离行为溢出效应和情境同伴效应。接着，研究者分析了个人及同伴的移动应用使用对学术成绩和劳动市场结果的影响，并探讨了这些影响的异质性。最后，研究者利用高频GPS数据和在线调查数据来探讨这些影响背后的机制。</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>乡村非农就业水平和农业技术采用情况</t>
+          <t>['移动应用使用具有传染性，室友的移动应用使用增加会导致个人使用增加。', '高移动应用使用对所有测量结果都是有害的，包括GPA和工资。', '室友的移动应用使用对个人的GPA和工资有直接和间接效应。', '限制未成年人游戏时间的政策可以提高大学生的初始工资。', '高频GPS数据显示，高应用使用挤出了学习时间和增加了迟到及缺课。']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>学术成绩（GPA）、劳动市场结果（工资）</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['农业发展水平', '产业结构', '政府规模', '金融发展水平', '固定资产投资水平', '人力资本水平', '交通基础设施水平', '通信基础设施水平']</t>
+          <t>个人及室友的移动应用使用时间</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>数据来源于农业农村部网站、国家统计局网站、各地方统计局和全球统计数据平台。</t>
+          <t>时间分配（学习时间、迟到和缺课）</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>使用农村居民人均纯收入的对数值作为被解释变量，控制变量包括农业发展水平、产业结构等。</t>
+          <t>未成年人游戏限制政策、爆款游戏“原神”发布时间</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>/* 基准回归模型 */
-reg Y DID Z' i.year, vce(cluster id)
-/* 平行趋势检验模型 */
-reg Y DID##c.year Z' i.year, vce(cluster id)
-/* 作用机理检验模型 - 就业效应 */
-reg Y DID Emp Z' i.year, vce(cluster id)
-/* 作用机理检验模型 - 技术效应 */
-reg Y DID Tech Z' i.year, vce(cluster id)
-/* 异质性分析模型 */
-reg Y DID##c.Spot DID##c.Cult Z' i.year, vce(cluster id)
-/* 其中 Y 为被解释变量，DID 为核心解释变量，Emp 和 Tech 分别为就业效应和技术效应的中介变量，Spot 和 Cult 为乡村旅游资源禀赋的代理变量，Z' 为控制变量，i.year 为年份固定效应，id 为县固定效应。*/</t>
+          <t>年龄、农村居住、高中理科/文科轨迹、大学入学考试成绩、房价（家庭财富代理变量）</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>中国一所大学的行政记录和手机使用数据，以及通过GPS系统和在线调查收集的补充数据。</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>通过手机记录测量移动应用使用时间，通过行政记录测量学术成绩和劳动市场结果。</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Abdulkadiroğlu, Atila, Joshua Angrist, and Parag Pathak, “The elite illusion: Achievement effects at Boston and New York exam schools,” Econometrica, 2014.
+Allcott, Hunt, Luca Braghieri, Sarah Eichmeyer, and Matthew Gentzkow, “The welfare effects of social media,” American Economic Review, 2020.
+Brock, William A and Steven N Durlauf, “A multinomial choice model with social interactions,” in “The Economy as an Evolving Complex System III,” Oxford University Press, New York, 2006.
+Sacerdote, Bruce, “Peer effects with random assignment: Results for Dartmouth roommates,” The Quarterly Journal of Economics, 2001.</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>* 以二元游戏限制政策作为工具变量的2SLS回归
+ivregress 2sls y x (z = iv), first
+* 以爆款游戏发布作为工具变量的2SLS回归
+ivregress 2sls y x (z = iv), first</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>党建引领村集体经济组织赋能...山东省招远市D村的实证调查_王惠林.pdf</t>
+          <t>2-中国造船业的产业政策实施.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>党建引领村集体经济组织赋能农民农村共同富裕的实践路径——基于山东省招远市D村的实证调查</t>
+          <t>工业政策实施：来自中国造船业的实证证据</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>村集体经济组织与农民农村共同富裕具有内在的逻辑关联。村集体经济组织的经济发展职能和共有共享的分配原则促进了农民生活的富裕富足；村集体经济组织的政治和治理服务职能为农户提供了生存和发展的基本保障，助推农村宜居宜业。现阶段，农民农村共同富裕主要面临土地细碎化制约农业规模化经营、农村公共品供给不足、小农户难以有效对接大市场和社会结构转型背景下如何重塑村庄生活共同体等现实难题。</t>
+          <t>Panle Jia Barwick, Myrto Kalouptsidi, Nahim Bin Zahur</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>本文的研究具有理论意义和实践意义。理论意义在于揭示村集体经济组织与农民农村共同富裕的内在关联性，实践意义在于为推进农民农村共同富裕、助力乡村振兴提供参考。</t>
+          <t>未提供</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>研究逻辑/流程包括理论论证村集体经济组织与农民农村共同富裕的内在关联性，结合山东省招远市D村的实证案例，系统探讨农民农村共同富裕所面临的现实难题、党建引领村集体经济组织赋能农民农村共同富裕的实践机制、路径等问题，并总结实践经验。</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>本文采用案例研究方法，以山东省招远市D村为实证调查对象，通过分析D村的具体情况，探讨党建引领下村集体经济组织如何赋能农民农村共同富裕的实践机制和路径。</t>
+          <t>工业政策在全球范围内被广泛使用。设计和实施这些政策是一项复杂的任务。本文评估了不同工业政策工具的长期绩效，包括生产补贴、投资补贴、进入补贴和整合政策。研究以中国造船业为目标，该行业在21世纪初占全球产量的不到10%，但在国家五年计划期间获得多项政策干预后，迅速成为全球领先的船舶生产国。然而，这一增长伴随着大量新企业的涌入，加剧了行业分散和低产能利用率问题。</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['村集体经济组织的经济发展职能和共有共享的分配原则能够最大程度地提高村民福利、收入，促进农民生活富裕富足。', '成员权利的平等性和对弱势群体的保护为村民提供了生存和发展的基本保障。', '村集体经济组织的治理和服务职能有助于推动乡村宜居宜业。', '山东省D村以党建为引领，充分发挥村集体经济组织在农民生产生活领域的统筹协调作用，通过统一流转土地承包经营权，改善农业生产条件，降低经营成本；优化农业生产服务，降低生产成本；塑造品牌效应，畅通销售渠道和重建村庄生活共同体，赋能农民农村共同富裕，获得了较好的经济、政治和社会效应。']</t>
+          <t>本文的理论意义在于提供了工业政策设计的微观基础，强调了企业异质性、商业周期和企业成本结构在政策设计中的关键作用。实践意义在于，通过评估中国造船业的工业政策，为其他国家制定和实施工业政策提供了经验和教训。</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>农民农村共同富裕</t>
+          <t>研究首先构建了一个包含动态和企业异质性的结构模型，然后使用1998至2014年的企业层面数据进行估计。研究的主要挑战是缺乏关于政府补贴性质的信息，因此通过比较政策实施前后中国企业的成本结构来恢复补贴的规模。接着，通过反事实分析评估中国工业政策的长期影响，并探讨不同政策工具的相对绩效。</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>村集体经济组织</t>
+          <t>研究使用动态模型估计企业进入、退出和资本投资的决策。模型中，企业在每个时期进行库诺竞争，选择生产量，然后决定是否退出以及在继续运营的情况下进行多少投资。潜在进入者基于预期的终身利润流和进入成本做出一次性进入决策。通过估计模型，研究评估了中国工业政策对全球造船业的长期影响，并探讨了不同政策工具的相对绩效。</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>党建引领</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+          <t>['中国政府的补贴政策大幅提高了中国在全球造船业的市场份额，但大部分增长来自于从其他国家企业抢夺业务。', '不同政策工具的绩效差异显著，生产和投资补贴相对于进入补贴更为有效。', '工业政策的有效性受到商业周期和企业效率异质性的影响，反周期政策的表现优于顺周期政策。', '政策通过整合和针对低成本企业进行补贴可以显著减少扭曲，但中国政府的实际白名单政策偏向于国有企业，牺牲了最有效率的企业。']</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>企业生产量、企业进入和退出决策、企业投资</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>生产补贴、投资补贴、进入补贴、整合政策</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>山东省招远市D村的实证调查数据。</t>
+          <t>市场需求、企业成本结构、企业异质性</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>通过实证调查D村的情况，分析村集体经济组织在农民农村共同富裕中的作用和影响。</t>
+          <t>无</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>/* 由于缺乏具体的定量数据和分析需求，无法提供具体的Stata代码。通常，对于案例研究方法，Stata代码主要用于数据处理和统计分析，而本文的研究方法更侧重于定性分析。 */</t>
+          <t>企业资本存量、企业积压订单、企业年龄、企业所有权状态、地区、企业规模</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>数据来源包括Clarksons的全球船厂季度信息数据库和中国国家统计局的制造业企业年度数据库。</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>使用企业层面数据，包括产量、资本存量、特征以及船舶市场价格。</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Johnson, 1982
+Ito, 1992
+Amsden, 1989
+Lane, 2022
+Stiglitz and Lin, 2013</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>* 由于Stata代码较长，以下为简化示例
+ reg y x1 x2, vce(cluster clustervar)
+ ivreg2 y (x1 x2) z (x3 x4), first
+ xtset panelvar timevar
+ xtreg y x1 x2, fe
+ * 更多复杂的动态面板数据模型和结构估计代码将根据具体方法论详细编写</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>小农户如何走向农业组织化经...—来自农民工回流农户的证据_肖剑.pdf</t>
+          <t>3-中国企业注册改革.pdf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>小农户如何走向农业组织化经营——来自农民工回流农户的证据</t>
+          <t>企业注册改革、市场周转与效率：中国的企业注册改革</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>本文探讨了农业组织化在中国式农业现代化中的重要性，并分析了回流农民工形成的农业人力资本补偿对推动小农户组织化由被动型向主动型转变的现实意义。文章利用2017年中国农村家庭追踪调查数据，实证分析了农民工回流对农业组织化经营的影响，发现农民工回流显著促进了农户的组织化经营，并改善了农户农业生产的契约化、合作化及分工化的程度。</t>
+          <t>Panle Jia Barwick, Luming Chen, Shanjun Li, Xiaobo Zhang</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>本文不仅丰富了关于人力资本对农户农业组织化参与影响的文献，还阐明了回流农户对于改造传统农业、推动农业组织化发展的重要作用，为小农户与现代农业发展有机衔接提供了政策思路。</t>
+          <t>八月 2024</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>研究首先提出了问题的背景和重要性，然后通过理论分析和研究假设，构建了Tobit模型和中介效应模型进行实证分析，最后对模型估计结果进行了讨论。</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>本文使用2017年中国农村家庭追踪调查数据，构建Tobit模型和中介效应模型，通过农民工回流对农业组织化经营的影响进行实证分析，并对结果进行稳健性检验和异质性分析。</t>
+          <t>尽管各国普遍存在市场准入管制，但对这些管制如何影响企业动态和生产力的全面评估却相对缺乏。本文考察了2012-2014年中国广东省的试点项目（后来成为全国政策），旨在降低企业注册成本，鼓励创业活动。利用企业注册和年度报告的行政数据，分析显示改革使制造业部门的企业进入增加了25%，退出增加了8.7%。改革后进入者的生产力比改革前提高了1.1%，可能原因是金融约束的放松和竞争的加剧。</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['农民工回流显著提高了农户组织化经营的程度。', '回流农民工的契约精神、合作意识和企业家精神是实现农业组织化经营的重要传导机制。', '外出务工时长、地点和工作性质的不同对农业组织化经营的影响存在差异性。']</t>
+          <t>本文不仅填补了有关进入管制对企业动态和生产力影响的文献空白，而且提供了中国大规模政策变化对企业层面影响的证据。研究结果对于理解市场准入改革的经济效应具有重要的理论和实践意义。</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>农业组织化经营程度：累计得到的农户农业组织化经营程度。</t>
+          <t>文章首先介绍了研究背景和数据来源，然后构建了实证模型，接着讨论了企业进入、退出、规模和生产力的结果，并总结了稳健性检验。最后，探讨了影响企业生产力提升的潜在渠道和宏观影响。</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>户主回流务农：户主是否回流务农（二值虚拟变量）。</t>
+          <t>本文采用差分法(DID)策略，利用中国广东省企业注册改革的渐进式推广，通过比较改革前后企业进入和退出的变化来评估改革的影响。同时，通过三重差分设计来评估不同行业和企业类型对改革的异质性反应。</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>契约精神、合作意识、企业家精神：表征农户的人力资本水平。</t>
+          <t>['企业注册改革显著增加了企业进入率和退出率，提高了市场周转率。', '改革后新进入企业的生产力提高了1.1%，表明更激烈的市场竞争和更优质的创业者进入市场。', '改革对不同类型企业和行业的效应存在异质性，私企和放松管制程度较高的行业受益更多。', '改革对提高企业生产力和宏观经济增长具有积极影响。']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>村域内除去自身以外的同村回流务农人数：作为农民工回流的工具变量。</t>
+          <t>因变量包括企业进入数量、退出情况、企业规模（如营收和资本）和企业生产力。</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>户主特征、家庭特征、经营特征、村庄特征以及省份虚拟变量。</t>
+          <t>自变量是改革实施的二元变量，表示是否在改革后的时间点。</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2017年中国农村家庭追踪调查数据。</t>
+          <t>机制变量包括企业融资来源、企业家特征和企业股权结构。</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>被解释变量从契约化、合作化以及分工化三个维度描述农户的组织化经营，解释变量包括户主回流务农和农户农民工回流（均为0、1离散变量）。</t>
+          <t>工具变量是改革实施的时间，利用城市间改革实施的时间差异作为工具变量。</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>/* Tobit模型 */
-tobit agricultural_organization i.returned##i.X, ll(0)
-/* 中介效应模型 */
-ivprobit contractual_spirit i.returned##i.X
-ivtobit agricultural_organization i.contractual_spirit##i.X
-/* 稳健性检验 */
-ivregress 2sls agricultural_organization (returned = instrument) i.X
-/* 异质性分析 */
-tobit agricultural_organization##i.migration_experience##i.X, ll(0)</t>
-        </is>
-      </c>
+          <t>控制变量包括企业年龄、企业所有权类型、城市-行业固定效应、城市-年份固定效应和行业-年份固定效应等。</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>数据来源包括广东省2009年1月至2016年12月的企业注册数据库、企业年度报告数据库和2018年中国创新与创业企业调查(ESIEC)。</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>企业进入和退出通过注册记录和年度报告数据进行测量。企业规模通过营收和资本来衡量，企业生产力通过Aw et al. (2011)和Peters et al. (2017)的方法进行结构性估计。</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Aghion, P., Burgess, R., Redding, S. J., and Zilibotti, F. (2008). The unequal effects of liberalization: Evidence from dismantling the license raj in india. American Economic Review, 98(4):1397–1412.
+Alfaro, L. and Chari, A. (2014). Deregulation, misallocation, and size: Evidence from india. The Journal of Law and Economics, 57(4):897–936.
+Asturias, J., Hur, S., Kehoe, T. J., and Ruhl, K. J. (2023). Firm entry and exit and aggregate growth. American Economic Journal: Macroeconomics, 15(1):48–105.
+Aw, B. Y., Roberts, M. J., and Xu, D. Y. (2011). R&amp;d investment, exporting, and productivity dynamics. American Economic Review, 101(4):1312–44.
+Baily, M. N., Hulten, C., Campbell, D., Bresnahan, T., and Caves, R. E. (1992). Productivity dynamics in manufacturing plants. Brookings Papers on Economic Activity. Microeconomics, 1992:187–267.</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>集体经营性建设用地入市增值...——基于文昌农民的问卷调查_刘民培.pdf</t>
+          <t>4-城市交通政策的经济影响.pdf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>集体经营性建设用地入市增值收益分配方式的影响因素分析——基于文昌农民的问卷调查</t>
+          <t>城市交通政策的经济影响与均衡排序</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>本文基于海南省文昌市对农民的调查问卷，旨在研究农民对收益分配方式的意愿及其影响因素，以期完善收益分配机制、推进入市改革。研究发现，近六成农民选择股权分配按期分红的增值收益分配方式，年龄越大、对集体经济组织满意度越高、愿意将增值收益分给政府的农民偏向于选择股权分配按期分红，而教育程度越高、主要收入来源为非农业工作的农民偏向于选择一次性资金补偿。</t>
+          <t>Panle Jia Barwick, Shanjun Li, Andrew Waxman, Jing Wu, Tianli Xia</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>本研究具有理论和实践双重意义。理论上，丰富了集体经营性建设用地入市增值收益分配方式的研究；实践上，为政策制定者提供了农民意愿和影响因素的实证依据，有助于制定更符合农民利益的政策。</t>
+          <t>Journal of Urban Economics</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>研究首先通过问卷调查收集数据，然后运用Logistic回归模型分析影响农民选择增值收益分配方式的因素，最后根据分析结果提出政策建议。</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>研究采用问卷调查和Logistic回归模型的方法。首先，通过问卷调查收集文昌市农民对于集体经营性建设用地入市增值收益分配方式的意愿和相关信息；其次，使用Logistic回归模型分析影响农民选择的因素；最后，根据回归结果提出政策建议。</t>
+          <t>交通在塑造城市空间结构和经济活动组织中起着关键作用。许多发展中国家由于快速城市化和机动化，加之基础设施不足，造成了前所未有的交通拥堵和严重的经济后果。全球各地政府实施了一系列政策，包括限行、公共交通投资、拥堵收费和汽油税等，以应对这些挑战。这些政策短期内在缓解拥堵方面的有效性，关键在于出行方式的可替代性和出行需求对通勤成本变化的敏感性。从中期到长期来看，这些政策可能会通过家庭调整居住地点对城市空间结构产生更广泛的影响。这种排序响应反过来可能影响交通政策在减少拥堵方面的有效性。此外，许多解决拥堵的政策具有分配后果。例如，收取通行费可能会加剧公平问题，因为低收入家庭在交通上的支出占收入比例更大。本文旨在理解城市交通政策的效率和公平影响，同时考虑排序响应和内生拥堵。</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['近六成农民倾向于选择股权分配按期分红的分配方式。', '农民对于收益分配方式的选择会由于不同的因素影响而改变。', '农民对入市政策的了解程度与其选择股权分配按期分红的方式相关性不强。']</t>
+          <t>本文的理论意义在于发展和估计了一个包含偏好异质性的住宅排序均衡模型，允许通过内生拥堵在住房地点和通勤决策之间进行一般均衡反馈。实践意义在于，模型能够预测在不同交通政策下的新均衡结果，包括出行方式选择、家庭位置、拥堵水平、房价和社会福利。</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>集体经营性建设用地增值收益分配方式，定义为农民选择一次性资金补偿（0）或股权分配按期分红（1）。</t>
+          <t>研究逻辑首先通过家庭旅行调查估计出行时间和货币成本的异质性偏好，然后利用估计参数和工作地点构建每个通勤者的“通勤便利”属性，并在第二步中估计家庭对房产属性的偏好。研究考虑了观察到的家庭异质性和解决潜在内生性问题。</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>包括年龄（age）、受教育程度（edu）、主要收入来源（income）、是否参与过集体重大事务投票（vote）、集体经济组织工作满意度（js）、对集体经营性建设用地入市分配政策了解程度（ud）、集体经营性建设用地入市增值收益是否应该分给政府（tb）。</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+          <t>首先，使用家庭旅行调查数据估计出行模式选择的参数，包括时间和货币成本偏好。其次，利用估计的参数和工作地点构建“通勤便利”属性，并在住房需求模型中使用该属性估计家庭对房产属性的偏好。最后，通过模拟不同交通政策下的均衡住宅排序和交通结果，分解福利效应。</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>['不同政策对居住地点的空间模式和均衡房价的影响不同，甚至有时相反。', '住宅排序可能加强或削弱交通政策的拥堵减少潜力。', '交通政策在总体和不同收入群体中产生不同的福利含义。']</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>通勤模式选择、住房位置选择</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>性别（gender）、户口状态（rs）、是否赞同集体经营性建设用地入市流转（agree）、分给政府的比例（prop）、对集体经营性建设用地政策了解渠道（uc）、对本集体的集体经营性建设用地收益分配政策满意程度（ps）。</t>
+          <t>交通政策（限行、拥堵收费、地铁扩张）</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>数据来源于作者对海南省文昌市开展过集体经营性建设用地入市的五个村庄进行的实地调研，共发出问卷221份，回收209份，有效问卷209份。</t>
+          <t>偏好异质性、内生拥堵</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>通过问卷调查的方式，收集农民的个人特征、对集体经济组织工作的认知、对集体经营性建设用地流转的态度等数据。</t>
+          <t>车牌摇号中奖概率（用于工具变量）</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>logit y age edu income vote js ud tb gender rs agree prop uc ps
- /* y: 被解释变量，代表农民选择集体经营性建设用地增值收益分配方式
-  age: 年龄
-  edu: 受教育程度
-  income: 主要收入来源
-  vote: 是否参与过集体重大事务投票
-  js: 集体经济组织工作满意度
-  ud: 对集体经营性建设用地入市分配政策了解程度
-  tb: 集体经营性建设用地入市增值收益是否应该分给政府
-  gender: 性别
-  rs: 户口状态
-  agree: 是否赞同集体经营性建设用地入市流转
-  prop: 分给政府的比例
-  uc: 对集体经营性建设用地政策了解渠道
-  ps: 对本集体的集体经营性建设用地收益分配政策满意程度 */</t>
+          <t>房产大小、年龄、街区地址、交易价格、日期、家庭收入、年龄、性别、婚姻状况、户籍状态等</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>北京家庭旅行调查（BHTS）2010年和2014年的数据，以及2006-2014年北京居民的主要政府抵押贷款计划中的住房交易数据。</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>使用家庭旅行调查数据和住房交易数据，构建包括家庭和工作地点、出行模式选择、住房属性等的综合数据集。</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Akbar, Prottoy, “Who Benefits from Faster Public Transit?”, 2020. Working Paper.
+Akbar, Prottoy A, Victor Couture, Gilles Duranton, and Adam Storeygard, “Mobility and Congestion in Urban India,” American Economic Review, 2023, 113 (4), 1083–1111.
+Anderson, Michael L, “Subways, strikes, and slowdowns: The impacts of public transit on traffic congestion,” The American Economic Review, 2014, 104 (9), 2763–2796.
+Gu, Yizhen, Naijia Guo, Jing Wu, and Ben Zou, “Home Location Choices and the Gender Commute Gap,” Journal of Human Resources, 2021, pp. 1020–11263R2.
+Hainmueller, Jens, “Entropy Balancing for Causal Effects: A Multivariate Reweighting Method to Produce Balanced Samples in Observational Studies,” Political Analysis, 2012, 20 (1), 25?46.</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5-污染信息的价值.pdf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>从雾到霾：污染信息的价值</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Panle Jia Barwick, Shanjun Li, Liguo Lin, Eric Zou</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Journal of Political Economy</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2013年，中国启动了一个具有里程碑意义的空气质量监测和实时数据公开项目，显著增加了公众获取和对污染信息的意识。该项目触发了一系列行为改变，如更强的避免户外污染暴露和增加防护产品支出。这些行为响应减轻了空气污染的死亡影响。保守估计表明，该计划的健康益处比成本高出一个数量级。研究突出了在经常遭受严重空气污染但缺乏污染数据收集和传播的发展中国家提高公众获取污染信息的好处。</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>本研究在理论和实践上都具有重要意义。理论上，它填补了关于发展中国家公民日常生活中收集和传播污染信息影响的知识空白。实践上，它为发展中国家公共资金在改善信息基础设施和满足基本医疗、营养、教育需求之间的竞争提供了见解。</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>研究逻辑分为两步。首先，记录公共空气质量信息广泛可用后污染信息可用性和公民意识的变化。其次，研究监测计划如何影响行为和健康结果，重点关注文献中的两个核心对象：避免行为和空气污染的健康影响。通过检查户外活动和健康结果如何响应短期污染波动来衡量这些对象，并估计监测计划如何改变这些波动。</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>本研究采用差分法，利用中国空气质量监测计划在不同城市的分阶段实施作为自然实验。研究构建了一个综合数据库，包括社会对空气污染的认知、卫星空气质量测量、经济活动和健康结果等丰富结果，覆盖监测计划前后的时期。</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>['监测计划显著提高了公众获取污染信息的途径，显著增加了家庭对污染问题的意识。', '信息获取和公众意识的变化触发了一系列行为变化，包括增加污染避免和防御性购买。', '监测计划有可能减轻严重空气污染的一些毁灭性健康后果。', '监测计划在提高健康结果方面的成本效益比非常高，是发展中国家记录的最成功的环境政策之一。']</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>户外活动频率、健康结果、空气净化器销售量</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>空气污染水平（以AOD表示）</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>污染信息的可用性和公民意识</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>无</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>城市固定效应、年份固定效应、周年份固定效应、城市特定时间趋势</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>包括社会对空气污染的认知、卫星空气质量测量、经济活动和健康结果等丰富结果，覆盖监测计划前后的时期。</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>使用AOD作为空气污染的代理，通过MODIS算法从NASA卫星获取。</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Stigler, 1961
+Ashenfelter and Greenstone, 2004
+Murphy and Topel, 2006
+Barwick et al., 2020
+Greenstone et al., 2022</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>* 差分法估计
+reg Outcomect Pollutionct##Postct, vce(cluster city)
+* 事件研究法估计
+reg Outcomect Pollutionct##c.q(), vce(cluster city)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: implement incremental update support for Excel results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,10 +539,8 @@
           <t>Quarterly Journal of Economics</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024</t>
-        </is>
+      <c r="E2" t="n">
+        <v>2024</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -642,10 +640,8 @@
           <t>未提供</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="E3" t="n">
+        <v>2023</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -748,10 +744,8 @@
           <t>八月 2024</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024</t>
-        </is>
+      <c r="E4" t="n">
+        <v>2024</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -845,10 +839,8 @@
           <t>Journal of Urban Economics</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024</t>
-        </is>
+      <c r="E5" t="n">
+        <v>2024</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -942,10 +934,8 @@
           <t>Journal of Political Economy</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="E6" t="n">
+        <v>2022</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1025,6 +1015,216 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6-NEW-新增测试论文.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>数字分心与同伴影响：移动应用使用对学术和劳动市场结果的影响</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Panle Jia Barwick, Siyu Chen, Chao Fu, Teng Li</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>未提供</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>未提供</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>随着移动电话的过度使用，尤其是青少年和年轻人，全球范围内的担忧不断增加。本文提供了首个关于个人和同伴移动应用使用如何影响学术表现、身体健康和劳动市场结果的全面证据。研究利用中国一所大学的行政数据和手机记录，通过随机室友分配和政策冲击，探讨了个人和同伴手机应用使用的影响。研究发现，高应用使用对所有衡量结果都有负面影响，室友的应用使用通过直接和间接效应对GPA和工资产生负面影响。</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>本研究不仅理论上拓展了对数字成瘾的理解，而且在实践上为制定减少移动应用过度使用的干预政策提供了依据。</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>研究首先通过随机室友分配来估计同伴效应，然后利用政策变化作为工具变量来分离行为溢出效应和情境同伴效应，最后探讨了这些效应对学术表现和劳动市场结果的影响。</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>研究使用了工具变量方法，包括未成年人游戏限制政策和爆款游戏“原神”发布日期作为工具变量，来估计移动应用使用对学术表现和劳动市场结果的影响。</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>['移动应用使用具有传染性，室友的应用使用增加会导致个人应用使用增加。', '高应用使用对学术表现和劳动市场结果有负面影响。', '室友的应用使用通过直接和间接效应对个人的GPA和工资产生负面影响。', '限制未成年人游戏时间的政策可以提高大学生的初始工资。', '应用使用通过时间分配影响学术表现，高应用使用导致学生在图书馆的时间减少，迟到和缺课增加。']</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>学术表现（GPA）、劳动市场结果（工资）</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>个人和室友的移动应用使用时间</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>时间分配（图书馆时间、宿舍时间）、迟到和缺课</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>未成年人游戏限制政策、爆款游戏“原神”发布日期</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>年龄、农村居住、高中理科/文科轨迹、大学入学考试成绩、房价（家庭财富代理）</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>中国一所大学的行政记录和手机使用数据，以及通过手机GPS系统收集的地理位置数据和在线调查。</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>移动应用使用时间通过手机记录的月度使用时间来衡量，GPA和工资通过学校行政记录来衡量。</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Abdulkadiroğlu, Atila, Joshua Angrist, and Parag Pathak, “The elite illusion: Achievement effects at Boston and New York exam schools,” Econometrica, 2014, 82 (1), 137–196.
+Allcott, Hunt, Luca Braghieri, Sarah Eichmeyer, and Matthew Gentzkow, “The welfare effects of social media,” American Economic Review, 2020, 110 (3), 629–676.
+Brock, William A and Steven N Durlauf, “A multinomial choice model with social interactions,” in “In: Blume, L., Durlauf, S. (Eds.), The Economy as an Evolving Complex System III,” Oxford University Press, New York, 2006.
+Sacerdote, Bruce, “Peer effects with random assignment: Results for Dartmouth roommates,” The Quarterly Journal of Economics, 2001, 116 (2), 681–704.</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>* 工具变量估计
+ivregress 2sls y x (z = w1 w2)
+* 随机效应模型
+xtreg y x, fe
+* 固定效应模型
+xtreg y x, re
+* 动态面板数据模型
+xtabond y L.y x, gmm(L.y, lag(2 3))
+* 事件研究
+gen timevar = _n
+reg y i.timevar##i.post</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6-空气污染的医疗成本.pdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>空气污染的医疗成本：来自世界最大支付网络的证据</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Panle Jia Barwick, Shanjun Li, Deyu Rao, Nahim Bin Zahur</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>未提供</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>本文利用2013-2015年中国信用卡和借记卡交易的全样本数据，首次对发展中国家PM2.5的医疗成本进行了全国性分析。研究利用PM2.5的远程传输产生的空间溢出效应来生成当地污染的外生变化，并采用灵活的分布滞后模型来半参数化地捕捉污染暴露的动态响应。分析显示，PM2.5对医疗支出有显著影响，无论是短期还是中期。PM2.5每减少10微克/立方米，年度医疗支出将减少超过92亿美元，约占中国年度医疗支出的1.5%。</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>本文的研究对于理解环境规制的总体效益中空气污染的死亡率和发病率影响至关重要。特别是在发展中国家，如中国和印度，由于经济发展压力和环境规制松懈，空气污染问题尤为严重。本文提供了发展中国家空气污染对健康支出影响的全国性分析，对于制定和评估环境政策具有重要的理论和实践意义。</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>本文首先介绍了研究背景和数据来源，然后详细描述了实证框架和识别策略。接着，文章展示了估计结果，并基于参数估计计算了发病率成本。最后，文章总结了研究发现，并讨论了其对环境政策的影响。</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>本文采用的主要方法是灵活的分布滞后模型，该模型扩展了Almon技术，并使用有限阶B样条函数灵活捕捉长滞后效应。结合IV方法解决同期和滞后空气污染测量的内生性问题。本文的方法是半参数化的，可以灵活适应各种数据模式。</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>['PM2.5对医疗支出有显著的短期和中期影响。', 'PM2.5每减少10微克/立方米，将减少超过92亿美元的年度医疗支出。', '空气污染的健康成本可能被低估，特别是对于发展中国家。', '本文提供了一种评估发展中国家空气污染健康影响的新方法。']</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>医疗支出（依赖变量：包括医疗交易频率和价值）</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>PM2.5浓度（独立变量：空气污染的度量）</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>污染暴露（机制变量：通过PM2.5的空间溢出效应来捕捉）</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>非本地源PM2.5浓度（工具变量：利用PM2.5的远程传输属性）</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>天气条件、节假日和工作日固定效应、季节性、城市特定时间趋势等</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>数据来源包括中国所有监测站的小时级空气污染读数、中国银联网络的信用卡和借记卡交易数据、国家海洋和大气管理局的气象数据。</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>使用城市日级别的数据，包括PM2.5浓度、医疗交易数量和价值、天气条件等。</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>ALMON, S. (1965): “The distributed lag between capital appropriations and expenditures,” Econometrica, 178–196.
+ANDERSON, M. L. (2020): “As the Wind Blows: The Effects of Long-Term Exposure to Air Pollution on Mortality,” Journal of the European Economic Association, 18, 1886–1927.
+ANDREWS, I., J. H. STOCK, AND L. SUN (2019): “Weak instruments in instrumental variables regression: Theory and practice,” Annual Review of Economics, 11, 727–753.
+*[其余参考文献列表省略]*</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>*[此处省略具体的Stata代码，因代码较长且需要根据具体方法论详细编写]*</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>